<commit_message>
thêm ứng viên ngày 27/08
</commit_message>
<xml_diff>
--- a/hồ sơ/tổng hợp_cv.xlsx
+++ b/hồ sơ/tổng hợp_cv.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="123">
   <si>
     <t>Họ Tên</t>
   </si>
@@ -289,13 +289,136 @@
   </si>
   <si>
     <t>Cty DeHa</t>
+  </si>
+  <si>
+    <t>TRƯƠNG QUANG THIỆU</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>thieutq.32@gmail.com</t>
+  </si>
+  <si>
+    <t>Chuyên viên PPBL</t>
+  </si>
+  <si>
+    <t>Cty IVT</t>
+  </si>
+  <si>
+    <t>9.000.000</t>
+  </si>
+  <si>
+    <t>PHẠM ĐÌNH LỘC</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>ph.dinhloc@gmail.com</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.000.000 </t>
+  </si>
+  <si>
+    <t>Đỗ Hoàng An</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>dohan9676@gmail.com</t>
+  </si>
+  <si>
+    <t>MKO</t>
+  </si>
+  <si>
+    <t>8.500.000 đ</t>
+  </si>
+  <si>
+    <t>Bùi Thị Lan Anh</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0982 997 692  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                         </t>
+    </r>
+  </si>
+  <si>
+    <t>lananhbui87@gmail.com</t>
+  </si>
+  <si>
+    <t>Trung tâm Thông tin- Ban Tôn giáo Chính phủ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bùi Thị Hảo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0982.507.740 </t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haohao591995.haui@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cty Kiến trúc Phong Thủy Tam Nguyên </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIỀU CÔNG QUẢNG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0969.000.960 </t>
+  </si>
+  <si>
+    <t>Chuyên viên Quản trị dự án</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cty viễn thống Quốc tế HTC-ITC </t>
+  </si>
+  <si>
+    <t>Phạm Thu Giang</t>
+  </si>
+  <si>
+    <t>Công ty Cổ phần JVB Việt Nam.</t>
+  </si>
+  <si>
+    <t>phamthugiang1706966@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kieucongquang@gmail.com </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,8 +494,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +512,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -430,6 +566,31 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -724,7 +885,7 @@
     <col min="3" max="3" width="29.140625" style="5"/>
     <col min="4" max="4" width="35.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="69.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" style="5" customWidth="1"/>
     <col min="7" max="16384" width="29.140625" style="5"/>
   </cols>
   <sheetData>
@@ -1110,7 +1271,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="5">
@@ -1130,13 +1291,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="10">
         <v>1991</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="17">
         <v>12999779</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -1153,13 +1314,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="21" t="s">
         <v>86</v>
       </c>
       <c r="B21" s="13">
         <v>1994</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="18">
         <v>366167337</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1170,6 +1331,161 @@
       </c>
       <c r="F21" s="5" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="19">
+        <v>983015619</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="19">
+        <v>912740868</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="19">
+        <v>837322100</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="24">
+        <v>901784108</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1181,8 +1497,10 @@
     <hyperlink ref="D10" r:id="rId4"/>
     <hyperlink ref="D14" r:id="rId5" display="mailto:xtho.lthuong@gmail.com"/>
     <hyperlink ref="D19" r:id="rId6"/>
+    <hyperlink ref="D28" r:id="rId7"/>
+    <hyperlink ref="D27" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>